<commit_message>
Final results for all configurations
</commit_message>
<xml_diff>
--- a/data/results/Topic_Model_Results.xlsx
+++ b/data/results/Topic_Model_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leer1\Documents\aaPERSONAL\School\CS678 (W2018)\topic-eval\data\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6CDF13-77DE-4B1C-A286-622900679E6F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C7B014-7495-4DEF-B070-4AB456529C7A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34560" windowHeight="15672" activeTab="1" xr2:uid="{BADD45CF-1CB1-4927-9369-96AB270861FF}"/>
   </bookViews>
@@ -803,7 +803,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Cleaned</a:t>
+              <a:t> Vocabulary Restricted</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -930,6 +930,1301 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
+              <c:f>Sheet1!$A$2:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>SAM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LDA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-166.0944672965</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-170.67072400400002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-16E7-4419-A55E-279691CB51D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>SAM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LDA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-291.88419422150002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-16E7-4419-A55E-279691CB51D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-158.79260302200001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-16E7-4419-A55E-279691CB51D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="326087184"/>
+        <c:axId val="326087512"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="326087184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="326087512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="326087512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Avg.</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Coherence Value (log)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="326087184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Newsgroups</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Raw</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SAM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>SAM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LDA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$A$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-147.39071374299999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-531C-4768-8655-58296F136EB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>LDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>SAM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>LDA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-166.8933403565</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-531C-4768-8655-58296F136EB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AW</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-132.812459265</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-531C-4768-8655-58296F136EB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="326087184"/>
+        <c:axId val="326087512"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="326087184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="326087512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="326087512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Avg.</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Coherence Value (log)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="326087184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Newsgroups Vocabulary Restricted</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SAM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
               <c:f>Sheet1!$F$2:$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
@@ -947,22 +2242,22 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$5</c:f>
+              <c:f>(Sheet2!$E$3,Sheet2!$I$3)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-166.0944672965</c:v>
+                  <c:v>-162.92898552399998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-170.67072400400002</c:v>
+                  <c:v>-389.55445713300003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A615-428D-9BA6-4A8AD744E521}"/>
+              <c16:uniqueId val="{00000000-0EC1-4E59-8CF0-0F997AD772E7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -971,7 +2266,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>Sheet2!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1068,19 +2363,19 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$3</c:f>
+              <c:f>Sheet2!$F$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-291.88419422150002</c:v>
+                  <c:v>-172.05435858850001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A615-428D-9BA6-4A8AD744E521}"/>
+              <c16:uniqueId val="{00000001-0EC1-4E59-8CF0-0F997AD772E7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1089,12 +2384,9 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$2</c:f>
+              <c:f>Sheet2!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>AW</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1169,19 +2461,19 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$3</c:f>
+              <c:f>Sheet2!$G$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>-158.79260302200001</c:v>
+                  <c:v>-147.44266935799999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A615-428D-9BA6-4A8AD744E521}"/>
+              <c16:uniqueId val="{00000002-0EC1-4E59-8CF0-0F997AD772E7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1490,6 +2782,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1994,6 +3366,1012 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2537,26 +4915,109 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>156210</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D31FE9AE-AE53-433F-B747-F03C4DD5D3EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A8345DE-6FF4-43CB-8745-3C7ACA238F15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B66DBFC6-4485-48AF-AB25-766039CE9238}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83DDDDE4-556F-4E0A-996F-8452C1376B3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2873,7 +5334,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3017,7 +5478,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3065,6 +5526,10 @@
         <f>AVERAGE(B5:B6)</f>
         <v>-166.8933403565</v>
       </c>
+      <c r="C3">
+        <f>AVERAGE(C5:C6)</f>
+        <v>-132.812459265</v>
+      </c>
       <c r="E3">
         <f>AVERAGE(E5:E6)</f>
         <v>-162.92898552399998</v>
@@ -3072,6 +5537,10 @@
       <c r="F3">
         <f>AVERAGE(F5:F6)</f>
         <v>-172.05435858850001</v>
+      </c>
+      <c r="G3">
+        <f>AVERAGE(G5:G6)</f>
+        <v>-147.44266935799999</v>
       </c>
       <c r="I3">
         <f>AVERAGE(I5:I6)</f>
@@ -3085,11 +5554,17 @@
       <c r="B5">
         <v>-166.03745821999999</v>
       </c>
+      <c r="C5">
+        <v>-132.812459265</v>
+      </c>
       <c r="E5">
         <v>-162.57418852699999</v>
       </c>
       <c r="F5">
         <v>-170.28767338700001</v>
+      </c>
+      <c r="G5">
+        <v>-145.878208626</v>
       </c>
       <c r="I5">
         <v>-390.112840576</v>
@@ -3102,11 +5577,17 @@
       <c r="B6">
         <v>-167.74922249299999</v>
       </c>
+      <c r="C6">
+        <v>-132.812459265</v>
+      </c>
       <c r="E6">
         <v>-163.28378252100001</v>
       </c>
       <c r="F6">
         <v>-173.82104379</v>
+      </c>
+      <c r="G6">
+        <v>-149.00713009</v>
       </c>
       <c r="I6">
         <v>-388.99607369</v>
@@ -3115,5 +5596,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Forgot to save spreadsheet before comitting
</commit_message>
<xml_diff>
--- a/data/results/Topic_Model_Results.xlsx
+++ b/data/results/Topic_Model_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leer1\Documents\aaPERSONAL\School\CS678 (W2018)\topic-eval\data\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C7B014-7495-4DEF-B070-4AB456529C7A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E30257-E889-47B9-B874-47E185754F64}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34560" windowHeight="15672" activeTab="1" xr2:uid="{BADD45CF-1CB1-4927-9369-96AB270861FF}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -5034,6 +5037,70 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="New Topics - LDA"/>
+      <sheetName val="Vocab pruning"/>
+      <sheetName val="New Topics - baseline (2)"/>
+      <sheetName val="FINAL"/>
+      <sheetName val="News Topics - clean (2)"/>
+      <sheetName val="News - tf_idf (2)"/>
+      <sheetName val="NEWS"/>
+      <sheetName val="ENRON"/>
+      <sheetName val="Enron Topics LDA"/>
+      <sheetName val="Enron Topics - baseline"/>
+      <sheetName val="Enron Topics - clean"/>
+      <sheetName val="Enron Topics - tf_idf"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6">
+        <row r="2">
+          <cell r="G2" t="str">
+            <v>SAM (ngrams)</v>
+          </cell>
+          <cell r="H2" t="str">
+            <v>SAM (tf-idf)</v>
+          </cell>
+          <cell r="I2" t="str">
+            <v>LDA</v>
+          </cell>
+          <cell r="J2" t="str">
+            <v>AW</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="G3">
+            <v>-169.8365704295</v>
+          </cell>
+          <cell r="H3">
+            <v>-199</v>
+          </cell>
+          <cell r="I3">
+            <v>-291.88419422150002</v>
+          </cell>
+          <cell r="J3">
+            <v>-158.79260302200001</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>

</xml_diff>